<commit_message>
Feb 16 2021 Update
</commit_message>
<xml_diff>
--- a/CAMCAR_COVID_Cases.xlsx
+++ b/CAMCAR_COVID_Cases.xlsx
@@ -55,10 +55,13 @@
     <t xml:space="preserve">Daily Incidence pct</t>
   </si>
   <si>
+    <t xml:space="preserve">Panama</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dominican Republic</t>
   </si>
   <si>
-    <t xml:space="preserve">Panama</t>
+    <t xml:space="preserve">Costa Rica</t>
   </si>
   <si>
     <t xml:space="preserve">Guatemala</t>
@@ -67,52 +70,49 @@
     <t xml:space="preserve">Honduras</t>
   </si>
   <si>
-    <t xml:space="preserve">Costa Rica</t>
-  </si>
-  <si>
     <t xml:space="preserve">El Salvador</t>
   </si>
   <si>
+    <t xml:space="preserve">Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica</t>
+  </si>
+  <si>
     <t xml:space="preserve">Haiti</t>
   </si>
   <si>
-    <t xml:space="preserve">Jamaica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuba</t>
+    <t xml:space="preserve">Bahamas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guyana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aruba</t>
   </si>
   <si>
     <t xml:space="preserve">Nicaragua</t>
   </si>
   <si>
-    <t xml:space="preserve">Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aruba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bahamas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guyana</t>
+    <t xml:space="preserve">Curacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Lucia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbados</t>
   </si>
   <si>
     <t xml:space="preserve">St Martin</t>
   </si>
   <si>
-    <t xml:space="preserve">Curacao</t>
+    <t xml:space="preserve">Antigua and Barbuda</t>
   </si>
   <si>
     <t xml:space="preserve">Cayman Islands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barbados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antigua and Barbuda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saint Lucia</t>
   </si>
 </sst>
 </file>
@@ -268,34 +268,34 @@
         <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>10847910</v>
+        <v>4314767</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>109737</v>
+        <v>332679</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2074</v>
+        <v>5642</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>83434</v>
+        <v>313783</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>24229</v>
+        <v>13254</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>468</v>
+        <v>500</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>0.019</v>
+        <v>0.017</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>1.89</v>
+        <v>1.696</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>1011.596</v>
+        <v>7710.243</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1.932</v>
+        <v>3.772</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,34 +303,34 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>4314767</v>
+        <v>10847910</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>107990</v>
+        <v>230563</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2291</v>
+        <v>2959</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>84437</v>
+        <v>178146</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>21262</v>
+        <v>49458</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>706</v>
+        <v>795</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0.021</v>
+        <v>0.013</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>2.121</v>
+        <v>1.283</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>2502.8</v>
+        <v>2125.414</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>3.32</v>
+        <v>1.607</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,34 +338,34 @@
         <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>17915568</v>
+        <v>5094118</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>87442</v>
+        <v>200024</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3154</v>
+        <v>2730</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>76459</v>
+        <v>163334</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>7829</v>
+        <v>33960</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>819</v>
+        <v>837</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.036</v>
+        <v>0.014</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>3.607</v>
+        <v>1.365</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>488.078</v>
+        <v>3926.568</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>10.461</v>
+        <v>2.465</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,34 +373,34 @@
         <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>9904607</v>
+        <v>17915568</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>72675</v>
+        <v>167383</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2222</v>
+        <v>6150</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>24022</v>
+        <v>154446</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>46431</v>
+        <v>6787</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>369</v>
+        <v>104</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.031</v>
+        <v>0.037</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>3.057</v>
+        <v>3.674</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>733.749</v>
+        <v>934.288</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.795</v>
+        <v>1.532</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,34 +408,34 @@
         <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>5094118</v>
+        <v>9904607</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>68059</v>
+        <v>160983</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>781</v>
+        <v>3893</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>26136</v>
+        <v>63346</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>41142</v>
+        <v>93744</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1370</v>
+        <v>812</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.011</v>
+        <v>0.024</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>1.148</v>
+        <v>2.418</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>1336.031</v>
+        <v>1625.335</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>3.33</v>
+        <v>0.866</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,31 +446,31 @@
         <v>6486205</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>27954</v>
+        <v>58023</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>819</v>
+        <v>1750</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>22113</v>
+        <v>52688</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5022</v>
+        <v>3585</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>2.93</v>
+        <v>3.016</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>430.976</v>
+        <v>894.56</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>0</v>
+        <v>16.597</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,34 +478,34 @@
         <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>11402528</v>
+        <v>11326616</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>8646</v>
+        <v>39004</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>6551</v>
+        <v>33776</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>1870</v>
+        <v>4959</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>13</v>
+        <v>715</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.026</v>
+        <v>0.007</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>2.602</v>
+        <v>0.69</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>75.825</v>
+        <v>344.357</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>0.695</v>
+        <v>14.418</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,31 +516,31 @@
         <v>2961167</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>5395</v>
+        <v>19305</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>76</v>
+        <v>378</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1444</v>
+        <v>12635</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3875</v>
+        <v>6292</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>125</v>
+        <v>270</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.014</v>
+        <v>0.02</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>1.409</v>
+        <v>1.958</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>182.192</v>
+        <v>651.939</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>3.226</v>
+        <v>4.291</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,34 +548,34 @@
         <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>11326616</v>
+        <v>11402528</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>5270</v>
+        <v>12143</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>118</v>
+        <v>247</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>4582</v>
+        <v>9354</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>570</v>
+        <v>2542</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.022</v>
+        <v>0.02</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>2.239</v>
+        <v>2.034</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>46.528</v>
+        <v>106.494</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>8.421</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,31 +583,31 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>6624554</v>
+        <v>393244</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>5073</v>
+        <v>8311</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2913</v>
+        <v>6931</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2011</v>
+        <v>1202</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.029</v>
+        <v>0.021</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>2.937</v>
+        <v>2.142</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>76.579</v>
+        <v>2113.446</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0</v>
@@ -618,34 +618,34 @@
         <v>21</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1399488</v>
+        <v>786552</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>4136</v>
+        <v>8232</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>67</v>
+        <v>186</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>1960</v>
+        <v>7399</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>2109</v>
+        <v>647</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.016</v>
+        <v>0.023</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>1.62</v>
+        <v>2.259</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>295.537</v>
+        <v>1046.593</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>5.216</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,34 +653,34 @@
         <v>22</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>106766</v>
+        <v>1399488</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>3721</v>
+        <v>7646</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>2501</v>
+        <v>7351</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>1195</v>
+        <v>157</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.007</v>
+        <v>0.018</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.672</v>
+        <v>1.805</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>3485.192</v>
+        <v>546.343</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>4.686</v>
+        <v>2.548</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,34 +688,34 @@
         <v>23</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>393244</v>
+        <v>106766</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3618</v>
+        <v>7438</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1915</v>
+        <v>7098</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>1623</v>
+        <v>272</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>151</v>
+        <v>25</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.022</v>
+        <v>0.009</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>2.211</v>
+        <v>0.914</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>920.039</v>
+        <v>6966.637</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>9.304</v>
+        <v>9.191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,34 +723,34 @@
         <v>24</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>786552</v>
+        <v>6624554</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>2535</v>
+        <v>6347</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1464</v>
+        <v>4225</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>1002</v>
+        <v>1951</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.027</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>2.722</v>
+        <v>2.694</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>322.293</v>
+        <v>95.81</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>9.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,34 +758,34 @@
         <v>25</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>38666</v>
+        <v>164093</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>367</v>
+        <v>4652</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>273</v>
+        <v>4571</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.022</v>
+        <v>0.005</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>2.18</v>
+        <v>0.473</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>949.154</v>
+        <v>2834.978</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>43.023</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,34 +793,34 @@
         <v>26</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>164093</v>
+        <v>183627</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>301</v>
+        <v>2519</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>104</v>
+        <v>1778</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>196</v>
+        <v>718</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.003</v>
+        <v>0.009</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0.332</v>
+        <v>0.913</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>183.433</v>
+        <v>1371.803</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>5.102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,34 +828,34 @@
         <v>27</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>65757</v>
+        <v>287375</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>210</v>
+        <v>2268</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>205</v>
+        <v>1639</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>4</v>
+        <v>605</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0</v>
+        <v>207</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.005</v>
+        <v>0.011</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>0.476</v>
+        <v>1.058</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>319.358</v>
+        <v>789.213</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0</v>
+        <v>34.215</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,31 +863,31 @@
         <v>28</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>287375</v>
+        <v>38666</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>189</v>
+        <v>1408</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>174</v>
+        <v>1050</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>8</v>
+        <v>346</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.037</v>
+        <v>0.009</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>3.704</v>
+        <v>0.852</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>65.768</v>
+        <v>3641.442</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>0</v>
@@ -901,31 +901,31 @@
         <v>97929</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>97</v>
+        <v>443</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>92</v>
+        <v>205</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>2</v>
+        <v>229</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.031</v>
+        <v>0.02</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>3.093</v>
+        <v>2.032</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>99.051</v>
+        <v>452.369</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>50</v>
+        <v>6.987</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,31 +933,31 @@
         <v>30</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>183627</v>
+        <v>65757</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>27</v>
+        <v>416</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>26</v>
+        <v>378</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>0</v>
+        <v>0.481</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>14.704</v>
+        <v>632.632</v>
       </c>
       <c r="K21" s="0" t="n">
         <v>0</v>

</xml_diff>